<commit_message>
Actualización del Contenido de los Juegos
</commit_message>
<xml_diff>
--- a/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
+++ b/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="45">
   <si>
     <t>x</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Representa el valor mínimo que haya en una muestra</t>
-  </si>
-  <si>
-    <t>Son todos los valores que se encuentran entre el mínimo y máximo de una muestra</t>
   </si>
   <si>
     <t>Es la suma de todos los valores de una muestra</t>
@@ -163,6 +160,12 @@
   </si>
   <si>
     <t>Agregaciones Segundo Nivel - Mundo</t>
+  </si>
+  <si>
+    <t>Son todos los valores que se encuentran entre el mínimo y máximo de una muestra.</t>
+  </si>
+  <si>
+    <t>Promedio Ponderado</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -629,7 +632,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -684,15 +687,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -711,9 +705,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -771,13 +762,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
@@ -825,7 +816,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,6 +846,20 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1181,10 +1186,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1224,7 +1229,7 @@
     </row>
     <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -1233,29 +1238,29 @@
         <v>13</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -1263,632 +1268,657 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6"/>
     <row r="11" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="25" t="s">
+      <c r="B11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="28" t="s">
+      <c r="H11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="57" t="s">
-        <v>26</v>
+      <c r="I11" s="53" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="58"/>
+      <c r="B12" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="30"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="54"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="43">
-        <v>1</v>
-      </c>
-      <c r="C13" s="36">
+      <c r="B13" s="39">
+        <v>1</v>
+      </c>
+      <c r="C13" s="32">
         <f>'Muestra - Extrema'!D16</f>
         <v>6</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="44">
         <f>'Muestra - Igualitaria'!D16</f>
         <v>0</v>
       </c>
-      <c r="E13" s="48">
+      <c r="E13" s="44">
         <f>'Muestra - Distribuida 1'!D16</f>
         <v>1</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="32">
         <f>'Muestra - Distribuida 2'!D16</f>
         <v>2</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="44">
         <f>SUM(C13:F13)</f>
         <v>9</v>
       </c>
-      <c r="H13" s="37">
+      <c r="H13" s="33">
         <f>+G13</f>
         <v>9</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="44">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="43">
+      <c r="B14" s="39">
         <v>2</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="32">
         <f>'Muestra - Extrema'!D17</f>
         <v>0</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="44">
         <f>'Muestra - Igualitaria'!D17</f>
         <v>0</v>
       </c>
-      <c r="E14" s="48">
+      <c r="E14" s="44">
         <f>'Muestra - Distribuida 1'!D17</f>
         <v>2</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="32">
         <f>'Muestra - Distribuida 2'!D17</f>
         <v>0</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="44">
         <f t="shared" ref="G14:G22" si="0">SUM(C14:F14)</f>
         <v>2</v>
       </c>
-      <c r="H14" s="37">
+      <c r="H14" s="33">
         <f>+G14+H13</f>
         <v>11</v>
       </c>
-      <c r="I14" s="48">
+      <c r="I14" s="44">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="43">
+      <c r="B15" s="39">
         <v>3</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="32">
         <f>'Muestra - Extrema'!D18</f>
         <v>0</v>
       </c>
-      <c r="D15" s="48">
+      <c r="D15" s="44">
         <f>'Muestra - Igualitaria'!D18</f>
         <v>0</v>
       </c>
-      <c r="E15" s="48">
+      <c r="E15" s="44">
         <f>'Muestra - Distribuida 1'!D18</f>
         <v>1</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="32">
         <f>'Muestra - Distribuida 2'!D18</f>
         <v>2</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="44">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H15" s="37">
+      <c r="H15" s="33">
         <f t="shared" ref="H15:H22" si="1">+G15+H14</f>
         <v>14</v>
       </c>
-      <c r="I15" s="48">
+      <c r="I15" s="44">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="43">
+      <c r="B16" s="39">
         <v>4</v>
       </c>
-      <c r="C16" s="36">
+      <c r="C16" s="32">
         <f>'Muestra - Extrema'!D19</f>
         <v>1</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="44">
         <f>'Muestra - Igualitaria'!D19</f>
         <v>0</v>
       </c>
-      <c r="E16" s="48">
+      <c r="E16" s="44">
         <f>'Muestra - Distribuida 1'!D19</f>
         <v>1</v>
       </c>
-      <c r="F16" s="36">
+      <c r="F16" s="32">
         <f>'Muestra - Distribuida 2'!D19</f>
         <v>0</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="44">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H16" s="37">
+      <c r="H16" s="33">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I16" s="48">
+      <c r="I16" s="44">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="43">
+      <c r="B17" s="39">
         <v>5</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="32">
         <f>'Muestra - Extrema'!D20</f>
         <v>0</v>
       </c>
-      <c r="D17" s="48">
+      <c r="D17" s="44">
         <f>'Muestra - Igualitaria'!D20</f>
         <v>0</v>
       </c>
-      <c r="E17" s="48">
+      <c r="E17" s="44">
         <f>'Muestra - Distribuida 1'!D20</f>
         <v>0</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="32">
         <f>'Muestra - Distribuida 2'!D20</f>
         <v>0</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H17" s="37">
+      <c r="H17" s="33">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I17" s="48">
+      <c r="I17" s="44">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="43">
+      <c r="B18" s="39">
         <v>6</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="32">
         <f>'Muestra - Extrema'!D21</f>
         <v>0</v>
       </c>
-      <c r="D18" s="48">
+      <c r="D18" s="44">
         <f>'Muestra - Igualitaria'!D21</f>
         <v>0</v>
       </c>
-      <c r="E18" s="48">
+      <c r="E18" s="44">
         <f>'Muestra - Distribuida 1'!D21</f>
         <v>0</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="32">
         <f>'Muestra - Distribuida 2'!D21</f>
         <v>1</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="44">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H18" s="37">
+      <c r="H18" s="33">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I18" s="48">
+      <c r="I18" s="44">
         <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="43">
+      <c r="B19" s="39">
         <v>7</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="32">
         <f>'Muestra - Extrema'!D22</f>
         <v>0</v>
       </c>
-      <c r="D19" s="48">
+      <c r="D19" s="44">
         <f>'Muestra - Igualitaria'!D22</f>
         <v>0</v>
       </c>
-      <c r="E19" s="48">
+      <c r="E19" s="44">
         <f>'Muestra - Distribuida 1'!D22</f>
         <v>0</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="32">
         <f>'Muestra - Distribuida 2'!D22</f>
         <v>1</v>
       </c>
-      <c r="G19" s="48">
+      <c r="G19" s="44">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="37">
+      <c r="H19" s="33">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="44">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="43">
+      <c r="B20" s="39">
         <v>8</v>
       </c>
-      <c r="C20" s="36">
+      <c r="C20" s="32">
         <f>'Muestra - Extrema'!D23</f>
         <v>0</v>
       </c>
-      <c r="D20" s="48">
+      <c r="D20" s="44">
         <f>'Muestra - Igualitaria'!D23</f>
         <v>0</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="44">
         <f>'Muestra - Distribuida 1'!D23</f>
         <v>2</v>
       </c>
-      <c r="F20" s="36">
+      <c r="F20" s="32">
         <f>'Muestra - Distribuida 2'!D23</f>
         <v>1</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="44">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H20" s="37">
+      <c r="H20" s="33">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I20" s="48">
+      <c r="I20" s="44">
         <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="43">
+      <c r="B21" s="39">
         <v>9</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="32">
         <f>'Muestra - Extrema'!D24</f>
         <v>0</v>
       </c>
-      <c r="D21" s="48">
+      <c r="D21" s="44">
         <f>'Muestra - Igualitaria'!D24</f>
         <v>0</v>
       </c>
-      <c r="E21" s="48">
+      <c r="E21" s="44">
         <f>'Muestra - Distribuida 1'!D24</f>
         <v>0</v>
       </c>
-      <c r="F21" s="36">
+      <c r="F21" s="32">
         <f>'Muestra - Distribuida 2'!D24</f>
         <v>0</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H21" s="37">
+      <c r="H21" s="33">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I21" s="48">
+      <c r="I21" s="44">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B22" s="43">
+      <c r="B22" s="39">
         <v>10</v>
       </c>
-      <c r="C22" s="36">
+      <c r="C22" s="32">
         <f>'Muestra - Extrema'!D25</f>
         <v>3</v>
       </c>
-      <c r="D22" s="48">
+      <c r="D22" s="44">
         <f>'Muestra - Igualitaria'!D25</f>
         <v>3</v>
       </c>
-      <c r="E22" s="48">
+      <c r="E22" s="44">
         <f>'Muestra - Distribuida 1'!D25</f>
         <v>0</v>
       </c>
-      <c r="F22" s="36">
+      <c r="F22" s="32">
         <f>'Muestra - Distribuida 2'!D25</f>
         <v>1</v>
       </c>
-      <c r="G22" s="48">
+      <c r="G22" s="44">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="H22" s="37">
+      <c r="H22" s="33">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I22" s="49">
+      <c r="I22" s="45">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B23" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>36</v>
+      <c r="B23" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B24" s="45" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="51">
+      <c r="B24" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="47">
         <f>'Muestra - Extrema'!H16</f>
         <v>1</v>
       </c>
-      <c r="D24" s="48">
+      <c r="D24" s="44">
         <f>'Muestra - Igualitaria'!H16</f>
         <v>10</v>
       </c>
-      <c r="E24" s="48">
+      <c r="E24" s="44">
         <f>'Muestra - Distribuida 1'!H16</f>
         <v>1</v>
       </c>
-      <c r="F24" s="59">
+      <c r="F24" s="55">
         <f>'Muestra - Distribuida 2'!H16</f>
         <v>1</v>
       </c>
-      <c r="G24" s="48">
+      <c r="G24" s="44">
         <f>MIN(B13:B22)</f>
         <v>1</v>
       </c>
-      <c r="H24" s="37"/>
+      <c r="H24" s="33"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B25" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="48">
+      <c r="B25" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="44">
         <f>'Muestra - Extrema'!H17</f>
         <v>10</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="44">
         <f>'Muestra - Igualitaria'!H17</f>
         <v>10</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="44">
         <f>'Muestra - Distribuida 1'!H17</f>
         <v>8</v>
       </c>
-      <c r="F25" s="59">
+      <c r="F25" s="55">
         <f>'Muestra - Distribuida 2'!H17</f>
         <v>10</v>
       </c>
-      <c r="G25" s="48">
+      <c r="G25" s="44">
         <f>MAX(B13:B22)</f>
         <v>10</v>
       </c>
-      <c r="H25" s="37"/>
+      <c r="H25" s="33"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="48">
+      <c r="C26" s="44">
         <f>'Muestra - Extrema'!H18</f>
         <v>40</v>
       </c>
-      <c r="D26" s="48">
+      <c r="D26" s="44">
         <f>'Muestra - Igualitaria'!H18</f>
         <v>30</v>
       </c>
-      <c r="E26" s="48">
+      <c r="E26" s="44">
         <f>'Muestra - Distribuida 1'!H18</f>
         <v>28</v>
       </c>
-      <c r="F26" s="59">
+      <c r="F26" s="55">
         <f>'Muestra - Distribuida 2'!H18</f>
         <v>39</v>
       </c>
-      <c r="G26" s="48">
+      <c r="G26" s="44">
         <f>+SUM(C26:F26)</f>
         <v>137</v>
       </c>
-      <c r="H26" s="37"/>
+      <c r="H26" s="33"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="44">
         <f>'Muestra - Extrema'!H19</f>
         <v>10</v>
       </c>
-      <c r="D27" s="48">
+      <c r="D27" s="44">
         <f>'Muestra - Igualitaria'!H19</f>
         <v>3</v>
       </c>
-      <c r="E27" s="48">
+      <c r="E27" s="44">
         <f>'Muestra - Distribuida 1'!H19</f>
         <v>7</v>
       </c>
-      <c r="F27" s="59">
+      <c r="F27" s="55">
         <f>'Muestra - Distribuida 2'!H19</f>
         <v>8</v>
       </c>
-      <c r="G27" s="48">
+      <c r="G27" s="44">
         <f>SUM(G13:G22)</f>
         <v>28</v>
       </c>
-      <c r="H27" s="37"/>
+      <c r="H27" s="33"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="60">
+      <c r="C28" s="56">
         <f>'Muestra - Extrema'!H20</f>
         <v>4</v>
       </c>
-      <c r="D28" s="60">
+      <c r="D28" s="56">
         <f>'Muestra - Igualitaria'!H20</f>
         <v>10</v>
       </c>
-      <c r="E28" s="60">
+      <c r="E28" s="56">
         <f>'Muestra - Distribuida 1'!H20</f>
         <v>4</v>
       </c>
-      <c r="F28" s="61">
+      <c r="F28" s="57">
         <f>'Muestra - Distribuida 2'!H20</f>
         <v>4.875</v>
       </c>
-      <c r="G28" s="62">
+      <c r="G28" s="58">
         <f>+G26/G27</f>
         <v>4.8928571428571432</v>
       </c>
-      <c r="H28" s="63">
+      <c r="H28" s="59">
         <f>AVERAGE(C28:F28)</f>
         <v>5.71875</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="60">
+      <c r="C29" s="56">
         <f>'Muestra - Extrema'!H21</f>
         <v>1</v>
       </c>
-      <c r="D29" s="60">
+      <c r="D29" s="56">
         <f>'Muestra - Igualitaria'!H21</f>
         <v>10</v>
       </c>
-      <c r="E29" s="60">
+      <c r="E29" s="56">
         <f>'Muestra - Distribuida 1'!H21</f>
         <v>3</v>
       </c>
-      <c r="F29" s="61">
+      <c r="F29" s="57">
         <f>'Muestra - Distribuida 2'!H21</f>
         <v>4.5</v>
       </c>
-      <c r="G29" s="60">
+      <c r="G29" s="56">
         <f>(3+4)/2</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="63"/>
+      <c r="H29" s="59"/>
     </row>
     <row r="30" spans="2:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="49">
+      <c r="C30" s="45">
         <f>'Muestra - Extrema'!H22</f>
         <v>1</v>
       </c>
-      <c r="D30" s="49">
+      <c r="D30" s="45">
         <f>'Muestra - Igualitaria'!H22</f>
         <v>10</v>
       </c>
-      <c r="E30" s="49">
+      <c r="E30" s="45">
         <f>'Muestra - Distribuida 1'!H22</f>
         <v>2</v>
       </c>
-      <c r="F30" s="64">
+      <c r="F30" s="60">
         <f>'Muestra - Distribuida 2'!H22</f>
         <v>1</v>
       </c>
-      <c r="G30" s="49">
+      <c r="G30" s="45">
         <f>VLOOKUP(MAX(G13:G22),G13:I22,3,)</f>
         <v>1</v>
       </c>
-      <c r="H30" s="41"/>
+      <c r="H30" s="37"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="35"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="47"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="39"/>
-      <c r="D31" s="73"/>
-      <c r="E31" s="73"/>
-      <c r="F31" s="73"/>
-      <c r="G31" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="51"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="69">
+      <c r="C32" s="65">
         <f>C27/$G$27</f>
         <v>0.35714285714285715</v>
       </c>
-      <c r="D32" s="74">
+      <c r="D32" s="70">
         <f t="shared" ref="D32:F32" si="2">D27/$G$27</f>
         <v>0.10714285714285714</v>
       </c>
-      <c r="E32" s="74">
+      <c r="E32" s="70">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="F32" s="74">
+      <c r="F32" s="70">
         <f t="shared" si="2"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="G32" s="70">
+      <c r="G32" s="66">
         <f>SUM(C32:F32)</f>
         <v>1</v>
       </c>
-      <c r="H32" s="48"/>
+      <c r="H32" s="44"/>
     </row>
     <row r="33" spans="2:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B33" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="71">
+      <c r="B33" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="67">
         <f>C26/$G$26</f>
         <v>0.29197080291970801</v>
       </c>
-      <c r="D33" s="75">
+      <c r="D33" s="71">
         <f t="shared" ref="D33:F33" si="3">D26/$G$26</f>
         <v>0.21897810218978103</v>
       </c>
-      <c r="E33" s="75">
+      <c r="E33" s="71">
         <f t="shared" si="3"/>
         <v>0.20437956204379562</v>
       </c>
-      <c r="F33" s="75">
+      <c r="F33" s="71">
         <f t="shared" si="3"/>
         <v>0.28467153284671531</v>
       </c>
-      <c r="G33" s="72">
+      <c r="G33" s="68">
         <f>SUM(C33:F33)</f>
         <v>1</v>
       </c>
-      <c r="H33" s="49"/>
+      <c r="H33" s="45"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" s="97" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="98">
+        <f>C32*C28</f>
+        <v>1.4285714285714286</v>
+      </c>
+      <c r="D35" s="98">
+        <f>D32*D28</f>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="E35" s="98">
+        <f>E32*E28</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="98">
+        <f>F32*F28</f>
+        <v>1.3928571428571428</v>
+      </c>
+      <c r="G35" s="98">
+        <f>SUM(C35:F35)</f>
+        <v>4.8928571428571423</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1917,246 +1947,246 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="25" t="s">
+      <c r="A1" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="D1" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="38"/>
+    </row>
+    <row r="3" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="77">
+        <v>1</v>
+      </c>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="87"/>
+    </row>
+    <row r="4" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="77">
+        <v>2</v>
+      </c>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="87"/>
+    </row>
+    <row r="5" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="77">
+        <v>3</v>
+      </c>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="87"/>
+    </row>
+    <row r="6" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="77">
+        <v>4</v>
+      </c>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="87"/>
+    </row>
+    <row r="7" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="77">
+        <v>5</v>
+      </c>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="87"/>
+    </row>
+    <row r="8" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="77">
+        <v>6</v>
+      </c>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="87"/>
+    </row>
+    <row r="9" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="77">
+        <v>7</v>
+      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="87"/>
+    </row>
+    <row r="10" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="77">
+        <v>8</v>
+      </c>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="87"/>
+    </row>
+    <row r="11" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="77">
+        <v>9</v>
+      </c>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="87"/>
+    </row>
+    <row r="12" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="77">
+        <v>10</v>
+      </c>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="87"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="40" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="40"/>
+    </row>
+    <row r="14" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" s="50" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="42" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="42"/>
-    </row>
-    <row r="3" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="81">
-        <v>1</v>
-      </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="91"/>
-    </row>
-    <row r="4" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="81">
-        <v>2</v>
-      </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="91"/>
-    </row>
-    <row r="5" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="81">
-        <v>3</v>
-      </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="86"/>
-      <c r="F5" s="91"/>
-    </row>
-    <row r="6" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="81">
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="88"/>
+    </row>
+    <row r="15" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="78" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="72"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="88"/>
+    </row>
+    <row r="16" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="91"/>
-    </row>
-    <row r="7" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="81">
+      <c r="B16" s="72"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="88"/>
+    </row>
+    <row r="17" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="78" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="72"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="88"/>
+    </row>
+    <row r="18" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="84"/>
+      <c r="F18" s="89"/>
+    </row>
+    <row r="19" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="91"/>
-    </row>
-    <row r="8" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="81">
-        <v>6</v>
-      </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="91"/>
-    </row>
-    <row r="9" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="81">
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="90"/>
+    </row>
+    <row r="20" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="91"/>
-    </row>
-    <row r="10" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="81">
-        <v>8</v>
-      </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="91"/>
-    </row>
-    <row r="11" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="81">
-        <v>9</v>
-      </c>
-      <c r="B11" s="77"/>
-      <c r="C11" s="77"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="91"/>
-    </row>
-    <row r="12" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="81">
-        <v>10</v>
-      </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="77"/>
-      <c r="D12" s="77"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="91"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="44" t="s">
+      <c r="B20" s="72"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="83"/>
+      <c r="F20" s="88"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="44"/>
-    </row>
-    <row r="14" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="82" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="92"/>
-    </row>
-    <row r="15" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="82" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="92"/>
-    </row>
-    <row r="16" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="82" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="87"/>
-      <c r="F16" s="92"/>
-    </row>
-    <row r="17" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="92"/>
-    </row>
-    <row r="18" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="82" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="88"/>
-      <c r="F18" s="93"/>
-    </row>
-    <row r="19" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="82" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="78"/>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="88"/>
-      <c r="F19" s="94"/>
-    </row>
-    <row r="20" spans="1:6" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="82" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="92"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="44" t="s">
+      <c r="B21" s="35"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="75" customFormat="1" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="79" customFormat="1" ht="35.049999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="83" t="s">
+      <c r="B22" s="76"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="91"/>
+    </row>
+    <row r="23" spans="1:6" s="75" customFormat="1" ht="35.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A23" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="89"/>
-      <c r="F22" s="95"/>
-    </row>
-    <row r="23" spans="1:6" s="79" customFormat="1" ht="35.049999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A23" s="84" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="85"/>
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="96"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2184,19 +2214,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="23"/>
-      <c r="B1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -2429,34 +2459,34 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="20">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21">
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>4</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>5</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="18">
         <v>6</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="18">
         <v>7</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="18">
         <v>8</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="18">
         <v>9</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>10</v>
       </c>
     </row>
@@ -2503,16 +2533,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="G15" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -2522,7 +2552,7 @@
         <f>+COUNTIF($B$13:$K$13,C16)</f>
         <v>6</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="62" t="s">
         <v>2</v>
       </c>
       <c r="H16">
@@ -2538,7 +2568,7 @@
         <f t="shared" ref="D17:D25" si="1">+COUNTIF($B$13:$K$13,C17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="62" t="s">
         <v>3</v>
       </c>
       <c r="H17">
@@ -2554,7 +2584,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="62" t="s">
         <v>4</v>
       </c>
       <c r="H18">
@@ -2570,10 +2600,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="61">
         <f>COUNT($B$13:$K$13)</f>
         <v>10</v>
       </c>
@@ -2586,7 +2616,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="62" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="2">
@@ -2602,7 +2632,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="62" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="2">
@@ -2618,10 +2648,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H22" s="61">
         <f>MODE($B$13:$K$13)</f>
         <v>1</v>
       </c>
@@ -2634,7 +2664,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G23" s="66"/>
+      <c r="G23" s="62"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C24">
@@ -2685,259 +2715,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="23"/>
-      <c r="B1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="B2" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15">
         <v>9</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="27" t="s">
+      <c r="B3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="15">
         <v>8</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="B4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="15">
         <v>7</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="B5" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="15">
         <v>6</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="27" t="s">
+      <c r="B6" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="15">
         <v>4</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="27" t="s">
+      <c r="B8" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="15">
         <v>3</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="27" t="s">
+      <c r="B9" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15">
         <v>2</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="B10" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>0</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
+      <c r="B11" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="20">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21">
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>4</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>5</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="18">
         <v>6</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="18">
         <v>7</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="18">
         <v>8</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="18">
         <v>9</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>10</v>
       </c>
     </row>
@@ -2984,16 +3014,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="G15" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3003,7 +3033,7 @@
         <f>+COUNTIF($B$13:$K$13,C16)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="62" t="s">
         <v>2</v>
       </c>
       <c r="H16">
@@ -3019,7 +3049,7 @@
         <f t="shared" ref="D17:D25" si="1">+COUNTIF($B$13:$K$13,C17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="62" t="s">
         <v>3</v>
       </c>
       <c r="H17">
@@ -3035,7 +3065,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="62" t="s">
         <v>4</v>
       </c>
       <c r="H18">
@@ -3051,10 +3081,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="61">
         <f>COUNT($B$13:$K$13)</f>
         <v>3</v>
       </c>
@@ -3067,7 +3097,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="62" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="2">
@@ -3083,7 +3113,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="62" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="2">
@@ -3099,10 +3129,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H22" s="61">
         <f>MODE($B$13:$K$13)</f>
         <v>10</v>
       </c>
@@ -3165,19 +3195,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="23"/>
-      <c r="B1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3190,9 +3220,9 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15">
@@ -3205,9 +3235,9 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="15">
@@ -3218,15 +3248,15 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
-      <c r="G4" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="G4" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="15">
@@ -3237,15 +3267,15 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
+      <c r="G5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="15">
@@ -3256,15 +3286,15 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
-      <c r="G6" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
+      <c r="G6" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15">
@@ -3275,15 +3305,15 @@
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="G7" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="15">
@@ -3293,18 +3323,18 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+      <c r="F8" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="15">
@@ -3313,107 +3343,107 @@
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
+      <c r="E9" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15">
         <v>2</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
+      <c r="C10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
+      <c r="B11" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="20">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21">
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>4</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>5</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="18">
         <v>6</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="18">
         <v>7</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="18">
         <v>8</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="18">
         <v>9</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>10</v>
       </c>
     </row>
@@ -3460,16 +3490,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="G15" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3479,7 +3509,7 @@
         <f>+COUNTIF($B$13:$K$13,C16)</f>
         <v>1</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="62" t="s">
         <v>2</v>
       </c>
       <c r="H16">
@@ -3495,7 +3525,7 @@
         <f t="shared" ref="D17:D25" si="1">+COUNTIF($B$13:$K$13,C17)</f>
         <v>2</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="62" t="s">
         <v>3</v>
       </c>
       <c r="H17">
@@ -3511,7 +3541,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="62" t="s">
         <v>4</v>
       </c>
       <c r="H18">
@@ -3527,10 +3557,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="61">
         <f>COUNT($B$13:$K$13)</f>
         <v>7</v>
       </c>
@@ -3543,7 +3573,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="62" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="2">
@@ -3559,7 +3589,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="62" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="2">
@@ -3575,10 +3605,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H22" s="61">
         <f>MODE($B$13:$K$13)</f>
         <v>2</v>
       </c>
@@ -3641,19 +3671,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="23"/>
-      <c r="B1" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="95"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3666,11 +3696,11 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
+      <c r="I2" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="15">
@@ -3683,11 +3713,11 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
+      <c r="I3" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="15">
@@ -3699,14 +3729,14 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
+      <c r="H4" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="15">
@@ -3717,17 +3747,17 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-      <c r="G5" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="33"/>
+      <c r="G5" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="15">
@@ -3737,20 +3767,20 @@
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="33"/>
+      <c r="F6" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="15">
@@ -3760,20 +3790,20 @@
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="33"/>
+      <c r="F7" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I7" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="15">
@@ -3783,20 +3813,20 @@
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="33"/>
+      <c r="F8" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="15">
@@ -3804,26 +3834,26 @@
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="33"/>
+      <c r="D9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="15">
@@ -3831,87 +3861,87 @@
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="33"/>
+      <c r="D10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A11" s="16">
         <v>1</v>
       </c>
-      <c r="B11" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="33"/>
+      <c r="B11" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B12" s="20">
-        <v>1</v>
-      </c>
-      <c r="C12" s="21">
+      <c r="B12" s="17">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18">
         <v>2</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="18">
         <v>3</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="18">
         <v>4</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="18">
         <v>5</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="18">
         <v>6</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="18">
         <v>7</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="18">
         <v>8</v>
       </c>
-      <c r="J12" s="21">
+      <c r="J12" s="18">
         <v>9</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="19">
         <v>10</v>
       </c>
     </row>
@@ -3958,16 +3988,16 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="30"/>
+      <c r="G15" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="96"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3977,7 +4007,7 @@
         <f>+COUNTIF($B$13:$K$13,C16)</f>
         <v>2</v>
       </c>
-      <c r="G16" s="66" t="s">
+      <c r="G16" s="62" t="s">
         <v>2</v>
       </c>
       <c r="H16">
@@ -3993,7 +4023,7 @@
         <f t="shared" ref="D17:D25" si="1">+COUNTIF($B$13:$K$13,C17)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="66" t="s">
+      <c r="G17" s="62" t="s">
         <v>3</v>
       </c>
       <c r="H17">
@@ -4009,7 +4039,7 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G18" s="66" t="s">
+      <c r="G18" s="62" t="s">
         <v>4</v>
       </c>
       <c r="H18">
@@ -4025,10 +4055,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="65">
+      <c r="H19" s="61">
         <f>COUNT($B$13:$K$13)</f>
         <v>8</v>
       </c>
@@ -4041,7 +4071,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G20" s="66" t="s">
+      <c r="G20" s="62" t="s">
         <v>6</v>
       </c>
       <c r="H20" s="2">
@@ -4057,7 +4087,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G21" s="66" t="s">
+      <c r="G21" s="62" t="s">
         <v>5</v>
       </c>
       <c r="H21" s="2">
@@ -4073,10 +4103,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G22" s="66" t="s">
+      <c r="G22" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="65">
+      <c r="H22" s="61">
         <f>MODE($B$13:$K$13)</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Revisión Inicial Semana 1 con Carolina
Incluye primera sesión de revisión e incorporación de comentarios a la semana 1.
</commit_message>
<xml_diff>
--- a/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
+++ b/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326" tabRatio="670" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Solucion de Juego" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="47">
   <si>
     <t>x</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Promedio Ponderado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bimodal </t>
+  </si>
+  <si>
+    <t>1 y 3</t>
   </si>
 </sst>
 </file>
@@ -632,7 +638,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -846,6 +852,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,8 +866,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1188,8 +1198,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1896,26 +1906,26 @@
       <c r="H33" s="45"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35" s="97" t="s">
+      <c r="B35" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="98">
+      <c r="C35" s="94">
         <f>C32*C28</f>
         <v>1.4285714285714286</v>
       </c>
-      <c r="D35" s="98">
+      <c r="D35" s="94">
         <f>D32*D28</f>
         <v>1.0714285714285714</v>
       </c>
-      <c r="E35" s="98">
+      <c r="E35" s="94">
         <f>E32*E28</f>
         <v>1</v>
       </c>
-      <c r="F35" s="98">
+      <c r="F35" s="94">
         <f>F32*F28</f>
         <v>1.3928571428571428</v>
       </c>
-      <c r="G35" s="98">
+      <c r="G35" s="94">
         <f>SUM(C35:F35)</f>
         <v>4.8928571428571423</v>
       </c>
@@ -1937,7 +1947,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2202,7 +2212,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2215,18 +2225,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -2539,10 +2549,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="96"/>
+      <c r="H15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -2702,7 +2712,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2716,18 +2726,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3020,10 +3030,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="96"/>
+      <c r="H15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3182,7 +3192,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3196,18 +3206,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3496,10 +3506,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="96"/>
+      <c r="H15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3657,8 +3667,8 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3672,18 +3682,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="93" t="s">
+      <c r="B1" s="95" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="94"/>
-      <c r="G1" s="94"/>
-      <c r="H1" s="94"/>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="95"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3994,10 +4004,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="96" t="s">
+      <c r="G15" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="96"/>
+      <c r="H15" s="98"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -4095,7 +4105,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C22">
         <v>7</v>
       </c>
@@ -4111,13 +4121,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="3:8" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C23">
         <v>8</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="G23" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="100" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Actualizacion presentaciones Lección 4
Presentaciones lección 4
</commit_message>
<xml_diff>
--- a/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
+++ b/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
@@ -9,16 +9,33 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326" tabRatio="670" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326" tabRatio="670"/>
   </bookViews>
   <sheets>
     <sheet name="Solucion de Juego" sheetId="1" r:id="rId1"/>
     <sheet name="Tablero de Juego" sheetId="17" r:id="rId2"/>
-    <sheet name="Muestra - Extrema" sheetId="2" r:id="rId3"/>
-    <sheet name="Muestra - Igualitaria" sheetId="14" r:id="rId4"/>
-    <sheet name="Muestra - Distribuida 1" sheetId="15" r:id="rId5"/>
-    <sheet name="Muestra - Distribuida 2" sheetId="16" r:id="rId6"/>
+    <sheet name="Histograma" sheetId="18" r:id="rId3"/>
+    <sheet name="Muestra - Extrema" sheetId="2" r:id="rId4"/>
+    <sheet name="Muestra - Igualitaria" sheetId="14" r:id="rId5"/>
+    <sheet name="Muestra - Distribuida 1" sheetId="15" r:id="rId6"/>
+    <sheet name="Muestra - Distribuida 2" sheetId="16" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Solucion de Juego'!$E$11</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Solucion de Juego'!$E$13:$E$22</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'Solucion de Juego'!$F$11</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'Solucion de Juego'!$F$13:$F$22</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Solucion de Juego'!$E$13:$E$22</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Solucion de Juego'!$C$11</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Solucion de Juego'!$D$11</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Solucion de Juego'!$D$13:$D$22</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -854,6 +871,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -864,10 +885,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -882,6 +899,7 @@
   <colors>
     <mruColors>
       <color rgb="FF808080"/>
+      <color rgb="FFF7B600"/>
       <color rgb="FFFF66FF"/>
     </mruColors>
   </colors>
@@ -894,6 +912,975 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Histograma</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Juego Lección 2.6</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Valores</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="F7B600"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="808080"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Solucion de Juego'!$G$13:$G$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A115-40F4-90E7-6D9D9BD495F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="572671040"/>
+        <c:axId val="567059056"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="572671040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="567059056"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="567059056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frecuencia</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572671040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="81" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9294519" cy="6072481"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD0654E-0690-4BBD-ABE3-12F1E1164485}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1198,8 +2185,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2225,18 +3212,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -2549,10 +3536,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="98"/>
+      <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -2726,18 +3713,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3030,10 +4017,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="98"/>
+      <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3206,18 +4193,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -3506,10 +4493,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="98"/>
+      <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -3667,8 +4654,8 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3682,18 +4669,18 @@
   <sheetData>
     <row r="1" spans="1:11" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A1" s="20"/>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="97"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="14">
@@ -4004,10 +4991,10 @@
       <c r="D15" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="98" t="s">
+      <c r="G15" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="98"/>
+      <c r="H15" s="100"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="C16">
@@ -4129,10 +5116,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G23" s="99" t="s">
+      <c r="G23" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="100" t="s">
+      <c r="H23" s="96" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizacion Presrntaciones Leccion 5
</commit_message>
<xml_diff>
--- a/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
+++ b/18-data-visualization/Contenido Semana 1/2.6. Muestras Poblacionales - Agregaciones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326" tabRatio="670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10326" tabRatio="670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Solucion de Juego" sheetId="1" r:id="rId1"/>
@@ -19,23 +19,8 @@
     <sheet name="Muestra - Igualitaria" sheetId="14" r:id="rId5"/>
     <sheet name="Muestra - Distribuida 1" sheetId="15" r:id="rId6"/>
     <sheet name="Muestra - Distribuida 2" sheetId="16" r:id="rId7"/>
+    <sheet name="Costos Legos" sheetId="19" r:id="rId8"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Solucion de Juego'!$E$11</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Solucion de Juego'!$E$13:$E$22</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'Solucion de Juego'!$F$11</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'Solucion de Juego'!$F$13:$F$22</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Solucion de Juego'!$B$13:$B$22</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Solucion de Juego'!$E$13:$E$22</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Solucion de Juego'!$C$11</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Solucion de Juego'!$C$13:$C$22</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Solucion de Juego'!$D$11</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Solucion de Juego'!$D$13:$D$22</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -47,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="62">
   <si>
     <t>x</t>
   </si>
@@ -189,6 +174,51 @@
   </si>
   <si>
     <t>1 y 3</t>
+  </si>
+  <si>
+    <t>Codigo Lego</t>
+  </si>
+  <si>
+    <t>Referencia Precio</t>
+  </si>
+  <si>
+    <t>Bases 12x12 para diseño</t>
+  </si>
+  <si>
+    <t>(Gris)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/LEGO-Classic-Green-Baseplate-Supplement/dp/B00NHQF65S/ref=sr_1_9?s=toys-and-games&amp;ie=UTF8&amp;qid=1500718895&amp;sr=1-9&amp;keywords=Lego</t>
+  </si>
+  <si>
+    <t>Bloques Rojos</t>
+  </si>
+  <si>
+    <t>https://shop.lego.com/en-US/</t>
+  </si>
+  <si>
+    <t>Bloques Verdes</t>
+  </si>
+  <si>
+    <t>Bloques Amarillos</t>
+  </si>
+  <si>
+    <t>Bloques Azules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOTAL </t>
+  </si>
+  <si>
+    <t># Grupos</t>
+  </si>
+  <si>
+    <t>Precio Unitario</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>ITEM</t>
   </si>
 </sst>
 </file>
@@ -199,7 +229,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +339,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -655,7 +691,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -886,6 +922,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2185,8 +2224,8 @@
   </sheetPr>
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView showGridLines="0" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2934,7 +2973,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3198,8 +3237,8 @@
   </sheetPr>
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5149,4 +5188,176 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="20.05078125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.47265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="138.20703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <f>+B11</f>
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>6.39</v>
+      </c>
+      <c r="D2">
+        <f>B2*C2</f>
+        <v>76.679999999999993</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3">
+        <f>40*$B$2</f>
+        <v>480</v>
+      </c>
+      <c r="C3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">B3*C3</f>
+        <v>67.2</v>
+      </c>
+      <c r="E3" s="101">
+        <v>300321</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4">
+        <f>40*$B$2</f>
+        <v>480</v>
+      </c>
+      <c r="C4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>67.2</v>
+      </c>
+      <c r="E4" s="101">
+        <v>300328</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5">
+        <f>40*$B$2</f>
+        <v>480</v>
+      </c>
+      <c r="C5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>67.2</v>
+      </c>
+      <c r="E5" s="101">
+        <v>300324</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6">
+        <f>40*$B$2</f>
+        <v>480</v>
+      </c>
+      <c r="C6">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>67.2</v>
+      </c>
+      <c r="E6" s="101">
+        <v>300323</v>
+      </c>
+      <c r="G6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <f>SUM(D2:D6)</f>
+        <v>345.47999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>